<commit_message>
Modificación para revisar rebase
</commit_message>
<xml_diff>
--- a/catkin_ws/src/icra2024/src/MDPs/policy_right_lane.xlsx
+++ b/catkin_ws/src/icra2024/src/MDPs/policy_right_lane.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1543" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1608" uniqueCount="56">
   <si>
     <t xml:space="preserve">Polìtica original V1</t>
   </si>
@@ -168,6 +168,9 @@
   </si>
   <si>
     <t xml:space="preserve"> sW2(0)=1) = change_lane</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Misma velocidad</t>
   </si>
   <si>
     <t xml:space="preserve"> free_SW(0)=0</t>
@@ -309,7 +312,7 @@
       <selection pane="topLeft" activeCell="O102" activeCellId="0" sqref="O102"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.29"/>
@@ -4973,21 +4976,31 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:D17"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="71" zoomScaleNormal="71" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G8" activeCellId="0" sqref="G8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="71" zoomScaleNormal="71" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I9" activeCellId="0" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="22.921875" defaultRowHeight="26.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="22.9140625" defaultRowHeight="26.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="38.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="3" width="30.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="29.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="29.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="29.16"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="5" style="3" width="22.89"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="5" style="3" width="22.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="3" width="36.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="3" width="29.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="3" width="29.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="3" width="27.98"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="11" style="3" width="22.89"/>
   </cols>
   <sheetData>
+    <row r="1" customFormat="false" ht="26.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G1" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
     <row r="2" customFormat="false" ht="26.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
         <v>21</v>
@@ -4996,10 +5009,22 @@
         <v>22</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D2" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>49</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="26.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5010,10 +5035,22 @@
         <v>22</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="26.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5024,10 +5061,22 @@
         <v>33</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D4" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I4" s="3" t="s">
         <v>49</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="26.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5038,10 +5087,22 @@
         <v>33</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="26.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5052,10 +5113,22 @@
         <v>22</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="26.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5066,10 +5139,22 @@
         <v>22</v>
       </c>
       <c r="C7" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>50</v>
+      <c r="G7" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="26.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5080,10 +5165,22 @@
         <v>33</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="26.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5094,10 +5191,22 @@
         <v>33</v>
       </c>
       <c r="C9" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>50</v>
+      <c r="G9" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="26.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5108,10 +5217,22 @@
         <v>22</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="26.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5122,10 +5243,22 @@
         <v>22</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="26.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5136,10 +5269,22 @@
         <v>33</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="26.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5150,10 +5295,22 @@
         <v>33</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="26.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5164,10 +5321,22 @@
         <v>22</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D14" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I14" s="3" t="s">
         <v>52</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="26.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5178,10 +5347,22 @@
         <v>22</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="26.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5192,10 +5373,22 @@
         <v>33</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="26.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5206,10 +5399,22 @@
         <v>33</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>